<commit_message>
Fixed - "None" in BF RR was converted to NaN in pandas
</commit_message>
<xml_diff>
--- a/inputs/en/demo_national_input.xlsx
+++ b/inputs/en/demo_national_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tharindu.wickram\Desktop\Modeling\Nutrition\inputs\en\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F249BD-1962-4D63-98FC-74DDB8594095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{041FF4DB-D184-4137-8E9F-699D30B95AC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="961" firstSheet="10" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="961" firstSheet="10" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
     <sheet name="Population risk areas" sheetId="64" state="hidden" r:id="rId19"/>
     <sheet name="IYCF odds ratios" sheetId="65" state="hidden" r:id="rId20"/>
     <sheet name="Birth outcome risks" sheetId="66" state="hidden" r:id="rId21"/>
-    <sheet name="Relative risks" sheetId="67" state="hidden" r:id="rId22"/>
+    <sheet name="Relative risks" sheetId="67" r:id="rId22"/>
     <sheet name="Odds ratios" sheetId="68" state="hidden" r:id="rId23"/>
     <sheet name="Programs birth outcomes" sheetId="69" state="hidden" r:id="rId24"/>
     <sheet name="Programs anaemia" sheetId="70" state="hidden" r:id="rId25"/>
@@ -6644,7 +6644,7 @@
   </sheetPr>
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -16870,6 +16870,42 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="z2Sh+MfQ/G4PueXRb8ZAtgj1nRGg65nslXBdmZZPRKgG1MxLre5J049ZmSpV+GTE/exeFs0taEhwHmOHXGbVug==" saltValue="5dHL9O3+Ennr8+ewoDPI6w==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="45">
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B55:B57"/>
+    <mergeCell ref="B58:B60"/>
+    <mergeCell ref="B61:B63"/>
+    <mergeCell ref="B64:B66"/>
+    <mergeCell ref="B67:B69"/>
+    <mergeCell ref="B72:B74"/>
+    <mergeCell ref="B75:B77"/>
+    <mergeCell ref="B78:B80"/>
+    <mergeCell ref="B81:B83"/>
+    <mergeCell ref="B84:B86"/>
+    <mergeCell ref="B108:B110"/>
+    <mergeCell ref="B89:B91"/>
+    <mergeCell ref="B92:B94"/>
+    <mergeCell ref="B95:B97"/>
+    <mergeCell ref="B98:B100"/>
+    <mergeCell ref="B101:B103"/>
+    <mergeCell ref="B111:B113"/>
+    <mergeCell ref="B114:B116"/>
+    <mergeCell ref="B117:B119"/>
+    <mergeCell ref="B120:B122"/>
+    <mergeCell ref="B125:B127"/>
     <mergeCell ref="B145:B147"/>
     <mergeCell ref="B148:B150"/>
     <mergeCell ref="B151:B153"/>
@@ -16879,42 +16915,6 @@
     <mergeCell ref="B134:B136"/>
     <mergeCell ref="B137:B139"/>
     <mergeCell ref="B142:B144"/>
-    <mergeCell ref="B111:B113"/>
-    <mergeCell ref="B114:B116"/>
-    <mergeCell ref="B117:B119"/>
-    <mergeCell ref="B120:B122"/>
-    <mergeCell ref="B125:B127"/>
-    <mergeCell ref="B108:B110"/>
-    <mergeCell ref="B89:B91"/>
-    <mergeCell ref="B92:B94"/>
-    <mergeCell ref="B95:B97"/>
-    <mergeCell ref="B98:B100"/>
-    <mergeCell ref="B101:B103"/>
-    <mergeCell ref="B72:B74"/>
-    <mergeCell ref="B75:B77"/>
-    <mergeCell ref="B78:B80"/>
-    <mergeCell ref="B81:B83"/>
-    <mergeCell ref="B84:B86"/>
-    <mergeCell ref="B55:B57"/>
-    <mergeCell ref="B58:B60"/>
-    <mergeCell ref="B61:B63"/>
-    <mergeCell ref="B64:B66"/>
-    <mergeCell ref="B67:B69"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -18150,8 +18150,8 @@
   </sheetPr>
   <dimension ref="A1:P328"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66:G101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -19855,16 +19855,16 @@
       <c r="C66" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="D66" s="103">
-        <v>1</v>
-      </c>
-      <c r="E66" s="103">
-        <v>1</v>
-      </c>
-      <c r="F66" s="103">
-        <v>1</v>
-      </c>
-      <c r="G66" s="103">
+      <c r="D66" s="104">
+        <v>1</v>
+      </c>
+      <c r="E66" s="104">
+        <v>1</v>
+      </c>
+      <c r="F66" s="104">
+        <v>1</v>
+      </c>
+      <c r="G66" s="104">
         <v>1</v>
       </c>
       <c r="H66" s="92">
@@ -19970,16 +19970,16 @@
       <c r="C70" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="D70" s="103">
-        <v>1</v>
-      </c>
-      <c r="E70" s="103">
-        <v>1</v>
-      </c>
-      <c r="F70" s="103">
-        <v>1</v>
-      </c>
-      <c r="G70" s="103">
+      <c r="D70" s="104">
+        <v>1</v>
+      </c>
+      <c r="E70" s="104">
+        <v>1</v>
+      </c>
+      <c r="F70" s="104">
+        <v>1</v>
+      </c>
+      <c r="G70" s="104">
         <v>1</v>
       </c>
       <c r="H70" s="92">
@@ -20085,16 +20085,16 @@
       <c r="C74" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="D74" s="103">
-        <v>1</v>
-      </c>
-      <c r="E74" s="103">
-        <v>1</v>
-      </c>
-      <c r="F74" s="103">
-        <v>1</v>
-      </c>
-      <c r="G74" s="103">
+      <c r="D74" s="104">
+        <v>1</v>
+      </c>
+      <c r="E74" s="104">
+        <v>1</v>
+      </c>
+      <c r="F74" s="104">
+        <v>1</v>
+      </c>
+      <c r="G74" s="104">
         <v>1</v>
       </c>
       <c r="H74" s="92">
@@ -20200,16 +20200,16 @@
       <c r="C78" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="D78" s="103">
-        <v>1</v>
-      </c>
-      <c r="E78" s="103">
-        <v>1</v>
-      </c>
-      <c r="F78" s="103">
-        <v>1</v>
-      </c>
-      <c r="G78" s="103">
+      <c r="D78" s="104">
+        <v>1</v>
+      </c>
+      <c r="E78" s="104">
+        <v>1</v>
+      </c>
+      <c r="F78" s="104">
+        <v>1</v>
+      </c>
+      <c r="G78" s="104">
         <v>1</v>
       </c>
       <c r="H78" s="92">
@@ -20315,16 +20315,16 @@
       <c r="C82" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="D82" s="103">
-        <v>1</v>
-      </c>
-      <c r="E82" s="103">
-        <v>1</v>
-      </c>
-      <c r="F82" s="103">
-        <v>1</v>
-      </c>
-      <c r="G82" s="103">
+      <c r="D82" s="104">
+        <v>1</v>
+      </c>
+      <c r="E82" s="104">
+        <v>1</v>
+      </c>
+      <c r="F82" s="104">
+        <v>1</v>
+      </c>
+      <c r="G82" s="104">
         <v>1</v>
       </c>
       <c r="H82" s="92">
@@ -20430,16 +20430,16 @@
       <c r="C86" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="D86" s="103">
-        <v>1</v>
-      </c>
-      <c r="E86" s="103">
-        <v>1</v>
-      </c>
-      <c r="F86" s="103">
-        <v>1</v>
-      </c>
-      <c r="G86" s="103">
+      <c r="D86" s="104">
+        <v>1</v>
+      </c>
+      <c r="E86" s="104">
+        <v>1</v>
+      </c>
+      <c r="F86" s="104">
+        <v>1</v>
+      </c>
+      <c r="G86" s="104">
         <v>1</v>
       </c>
       <c r="H86" s="92">
@@ -20545,16 +20545,16 @@
       <c r="C90" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="D90" s="103">
-        <v>1</v>
-      </c>
-      <c r="E90" s="103">
-        <v>1</v>
-      </c>
-      <c r="F90" s="103">
-        <v>1</v>
-      </c>
-      <c r="G90" s="103">
+      <c r="D90" s="104">
+        <v>1</v>
+      </c>
+      <c r="E90" s="104">
+        <v>1</v>
+      </c>
+      <c r="F90" s="104">
+        <v>1</v>
+      </c>
+      <c r="G90" s="104">
         <v>1</v>
       </c>
       <c r="H90" s="92">
@@ -20660,16 +20660,16 @@
       <c r="C94" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="D94" s="103">
-        <v>1</v>
-      </c>
-      <c r="E94" s="103">
-        <v>1</v>
-      </c>
-      <c r="F94" s="103">
-        <v>1</v>
-      </c>
-      <c r="G94" s="103">
+      <c r="D94" s="104">
+        <v>1</v>
+      </c>
+      <c r="E94" s="104">
+        <v>1</v>
+      </c>
+      <c r="F94" s="104">
+        <v>1</v>
+      </c>
+      <c r="G94" s="104">
         <v>1</v>
       </c>
       <c r="H94" s="92">
@@ -20775,16 +20775,16 @@
       <c r="C98" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="D98" s="103">
-        <v>1</v>
-      </c>
-      <c r="E98" s="103">
-        <v>1</v>
-      </c>
-      <c r="F98" s="103">
-        <v>1</v>
-      </c>
-      <c r="G98" s="103">
+      <c r="D98" s="104">
+        <v>1</v>
+      </c>
+      <c r="E98" s="104">
+        <v>1</v>
+      </c>
+      <c r="F98" s="104">
+        <v>1</v>
+      </c>
+      <c r="G98" s="104">
         <v>1</v>
       </c>
       <c r="H98" s="92">
@@ -26275,7 +26275,7 @@
       <c r="I328" s="92"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="DX2074WdMrLoNH6fB/42y5tQZ/0A6ySjvazKgvpMJtTZUgvKYbirYKOqPx9qaReeM6SxVleQ/wPqkd35PeIvNA==" saltValue="V2lMYpCQ/nr1EfnOt5Y4/Q==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection selectLockedCells="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
Only English LiST databooks in this push
</commit_message>
<xml_diff>
--- a/inputs/en/demo_national_input.xlsx
+++ b/inputs/en/demo_national_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tharindu.wickram\Desktop\Modeling\Nutrition\inputs\en\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{041FF4DB-D184-4137-8E9F-699D30B95AC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A51D3D52-7B53-47BC-90A9-520C4233362D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="961" firstSheet="10" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="961" firstSheet="6" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -32,10 +32,10 @@
     <sheet name="Programs impacted population" sheetId="62" state="hidden" r:id="rId17"/>
     <sheet name="Program risk areas" sheetId="63" state="hidden" r:id="rId18"/>
     <sheet name="Population risk areas" sheetId="64" state="hidden" r:id="rId19"/>
-    <sheet name="IYCF odds ratios" sheetId="65" state="hidden" r:id="rId20"/>
+    <sheet name="IYCF odds ratios" sheetId="65" r:id="rId20"/>
     <sheet name="Birth outcome risks" sheetId="66" state="hidden" r:id="rId21"/>
     <sheet name="Relative risks" sheetId="67" r:id="rId22"/>
-    <sheet name="Odds ratios" sheetId="68" state="hidden" r:id="rId23"/>
+    <sheet name="Odds ratios" sheetId="68" r:id="rId23"/>
     <sheet name="Programs birth outcomes" sheetId="69" state="hidden" r:id="rId24"/>
     <sheet name="Programs anaemia" sheetId="70" state="hidden" r:id="rId25"/>
     <sheet name="Programs wasting" sheetId="71" state="hidden" r:id="rId26"/>
@@ -18150,8 +18150,8 @@
   </sheetPr>
   <dimension ref="A1:P328"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66:G101"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H65" sqref="H65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -19855,16 +19855,16 @@
       <c r="C66" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="D66" s="104">
-        <v>1</v>
-      </c>
-      <c r="E66" s="104">
-        <v>1</v>
-      </c>
-      <c r="F66" s="104">
-        <v>1</v>
-      </c>
-      <c r="G66" s="104">
+      <c r="D66" s="103">
+        <v>1</v>
+      </c>
+      <c r="E66" s="103">
+        <v>1</v>
+      </c>
+      <c r="F66" s="103">
+        <v>1</v>
+      </c>
+      <c r="G66" s="103">
         <v>1</v>
       </c>
       <c r="H66" s="92">
@@ -19970,16 +19970,16 @@
       <c r="C70" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="D70" s="104">
-        <v>1</v>
-      </c>
-      <c r="E70" s="104">
-        <v>1</v>
-      </c>
-      <c r="F70" s="104">
-        <v>1</v>
-      </c>
-      <c r="G70" s="104">
+      <c r="D70" s="103">
+        <v>1</v>
+      </c>
+      <c r="E70" s="103">
+        <v>1</v>
+      </c>
+      <c r="F70" s="103">
+        <v>1</v>
+      </c>
+      <c r="G70" s="103">
         <v>1</v>
       </c>
       <c r="H70" s="92">
@@ -20085,16 +20085,16 @@
       <c r="C74" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="D74" s="104">
-        <v>1</v>
-      </c>
-      <c r="E74" s="104">
-        <v>1</v>
-      </c>
-      <c r="F74" s="104">
-        <v>1</v>
-      </c>
-      <c r="G74" s="104">
+      <c r="D74" s="103">
+        <v>1</v>
+      </c>
+      <c r="E74" s="103">
+        <v>1</v>
+      </c>
+      <c r="F74" s="103">
+        <v>1</v>
+      </c>
+      <c r="G74" s="103">
         <v>1</v>
       </c>
       <c r="H74" s="92">
@@ -20200,16 +20200,16 @@
       <c r="C78" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="D78" s="104">
-        <v>1</v>
-      </c>
-      <c r="E78" s="104">
-        <v>1</v>
-      </c>
-      <c r="F78" s="104">
-        <v>1</v>
-      </c>
-      <c r="G78" s="104">
+      <c r="D78" s="103">
+        <v>1</v>
+      </c>
+      <c r="E78" s="103">
+        <v>1</v>
+      </c>
+      <c r="F78" s="103">
+        <v>1</v>
+      </c>
+      <c r="G78" s="103">
         <v>1</v>
       </c>
       <c r="H78" s="92">
@@ -20315,16 +20315,16 @@
       <c r="C82" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="D82" s="104">
-        <v>1</v>
-      </c>
-      <c r="E82" s="104">
-        <v>1</v>
-      </c>
-      <c r="F82" s="104">
-        <v>1</v>
-      </c>
-      <c r="G82" s="104">
+      <c r="D82" s="103">
+        <v>1</v>
+      </c>
+      <c r="E82" s="103">
+        <v>1</v>
+      </c>
+      <c r="F82" s="103">
+        <v>1</v>
+      </c>
+      <c r="G82" s="103">
         <v>1</v>
       </c>
       <c r="H82" s="92">
@@ -20430,16 +20430,16 @@
       <c r="C86" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="D86" s="104">
-        <v>1</v>
-      </c>
-      <c r="E86" s="104">
-        <v>1</v>
-      </c>
-      <c r="F86" s="104">
-        <v>1</v>
-      </c>
-      <c r="G86" s="104">
+      <c r="D86" s="103">
+        <v>1</v>
+      </c>
+      <c r="E86" s="103">
+        <v>1</v>
+      </c>
+      <c r="F86" s="103">
+        <v>1</v>
+      </c>
+      <c r="G86" s="103">
         <v>1</v>
       </c>
       <c r="H86" s="92">
@@ -20545,16 +20545,16 @@
       <c r="C90" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="D90" s="104">
-        <v>1</v>
-      </c>
-      <c r="E90" s="104">
-        <v>1</v>
-      </c>
-      <c r="F90" s="104">
-        <v>1</v>
-      </c>
-      <c r="G90" s="104">
+      <c r="D90" s="103">
+        <v>1</v>
+      </c>
+      <c r="E90" s="103">
+        <v>1</v>
+      </c>
+      <c r="F90" s="103">
+        <v>1</v>
+      </c>
+      <c r="G90" s="103">
         <v>1</v>
       </c>
       <c r="H90" s="92">
@@ -20660,16 +20660,16 @@
       <c r="C94" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="D94" s="104">
-        <v>1</v>
-      </c>
-      <c r="E94" s="104">
-        <v>1</v>
-      </c>
-      <c r="F94" s="104">
-        <v>1</v>
-      </c>
-      <c r="G94" s="104">
+      <c r="D94" s="103">
+        <v>1</v>
+      </c>
+      <c r="E94" s="103">
+        <v>1</v>
+      </c>
+      <c r="F94" s="103">
+        <v>1</v>
+      </c>
+      <c r="G94" s="103">
         <v>1</v>
       </c>
       <c r="H94" s="92">
@@ -20775,16 +20775,16 @@
       <c r="C98" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="D98" s="104">
-        <v>1</v>
-      </c>
-      <c r="E98" s="104">
-        <v>1</v>
-      </c>
-      <c r="F98" s="104">
-        <v>1</v>
-      </c>
-      <c r="G98" s="104">
+      <c r="D98" s="103">
+        <v>1</v>
+      </c>
+      <c r="E98" s="103">
+        <v>1</v>
+      </c>
+      <c r="F98" s="103">
+        <v>1</v>
+      </c>
+      <c r="G98" s="103">
         <v>1</v>
       </c>
       <c r="H98" s="92">
@@ -26291,7 +26291,7 @@
   </sheetPr>
   <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>

</xml_diff>